<commit_message>
Added _11growthstg_clean, defaults to 7, if _11growthstg has no value. Extracted weather variables based on (_07pdate + _11growthstg_clean). Updated utils.addmonths, parsed n months to integer. Updated data dictionary.
</commit_message>
<xml_diff>
--- a/docs/app_data_dictionary_20180713.xlsx
+++ b/docs/app_data_dictionary_20180713.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAB\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAB\Data\dextraction\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="231">
   <si>
     <t>_plotno</t>
   </si>
@@ -678,7 +678,46 @@
     <t>Data Type</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>w_growthstg_date</t>
+  </si>
+  <si>
+    <t>11_growthstg_clean</t>
+  </si>
+  <si>
+    <t>Date where PD was observed (_07pdate + _11growthstg_clean)</t>
+  </si>
+  <si>
+    <t>cleaned version of _11growthstg (number of months after planting where P&amp;D was observed. Defaults to "7" if _11growthstg cannot be recalled)</t>
+  </si>
+  <si>
+    <t>Miscellaneous Variables</t>
+  </si>
+  <si>
+    <t>_map</t>
+  </si>
+  <si>
+    <t>_yr_obs</t>
+  </si>
+  <si>
+    <t>Number of months after planting (when crop is harvested)</t>
+  </si>
+  <si>
+    <t>Year for which the P&amp;D was observed (from w_growthstg_date)</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>Weather cell id column</t>
+  </si>
+  <si>
+    <t>Weather cell id row</t>
+  </si>
+  <si>
+    <t>Date (yyyy-mm-dd), but defaults to (mm/dd/yyyy) when opened in Excel</t>
   </si>
 </sst>
 </file>
@@ -722,7 +761,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -732,6 +771,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -846,50 +897,83 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,25 +1255,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:C38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
     <col min="2" max="2" width="67.140625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="18" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1198,10 +1282,10 @@
       <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="17" t="s">
         <v>216</v>
       </c>
     </row>
@@ -1212,8 +1296,8 @@
       <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1224,8 +1308,8 @@
       <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="30" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="21" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1236,8 +1320,8 @@
       <c r="B5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="30" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="21" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1248,20 +1332,20 @@
       <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="28"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1270,10 +1354,10 @@
       <c r="B9" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="17" t="s">
         <v>216</v>
       </c>
     </row>
@@ -1284,8 +1368,8 @@
       <c r="B10" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="21" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1296,10 +1380,10 @@
       <c r="B11" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1310,10 +1394,10 @@
       <c r="B12" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1324,10 +1408,10 @@
       <c r="B13" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1338,8 +1422,8 @@
       <c r="B14" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="30" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1350,7 +1434,7 @@
       <c r="B15" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="20" t="s">
         <v>206</v>
       </c>
     </row>
@@ -1361,8 +1445,8 @@
       <c r="B16" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30" t="s">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1373,8 +1457,8 @@
       <c r="B17" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1385,8 +1469,8 @@
       <c r="B18" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="21" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1397,740 +1481,841 @@
       <c r="B19" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="30"/>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="27"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C23" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D23" s="17" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B28" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>199</v>
+        <v>45</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="C29" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>207</v>
+        <v>203</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C30" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="21" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B33" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="C33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B35" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="19" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B37" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="28"/>
-      <c r="D37" s="30"/>
-    </row>
-    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="C37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="19"/>
+      <c r="D38" s="21"/>
+    </row>
+    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="19"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="B39" s="27"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B40" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C40" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D39" s="26" t="s">
+      <c r="D40" s="17" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="30" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="30" t="s">
+        <v>212</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B43" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="C43" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="28"/>
-      <c r="D44" s="30" t="s">
+      <c r="C44" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="19"/>
+      <c r="D45" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C46" s="28"/>
-      <c r="D46" s="30"/>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="19"/>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="19"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="B48" s="27"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B49" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C49" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D49" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="30" t="s">
+      <c r="C50" s="19"/>
+      <c r="D50" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B53" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="30" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="19"/>
+      <c r="D54" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B55" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="28"/>
-      <c r="D54" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B56" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="28"/>
-      <c r="D55" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" s="28"/>
-      <c r="D56" s="30" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B58" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+      <c r="C58" s="19"/>
+      <c r="D58" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B61" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C60" s="26" t="s">
+      <c r="C61" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="D61" s="17" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C61" s="28"/>
-      <c r="D61" s="30" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="19"/>
+      <c r="D62" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B63" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C62" s="28"/>
-      <c r="D62" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
+      <c r="C63" s="19"/>
+      <c r="D63" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B64" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C63" s="28"/>
-      <c r="D63" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="28"/>
-      <c r="D64" s="30" t="s">
+      <c r="C64" s="19"/>
+      <c r="D64" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="28"/>
-      <c r="D65" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B66" s="12" t="s">
+      <c r="B67" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C66" s="28"/>
-      <c r="D66" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B67" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="30" t="s">
+      <c r="C67" s="19"/>
+      <c r="D67" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C69" s="28"/>
-      <c r="D69" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B71" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
+      <c r="C71" s="19"/>
+      <c r="D71" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B72" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C71" s="28"/>
-      <c r="D71" s="30" t="s">
+      <c r="C72" s="19"/>
+      <c r="D72" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
+    <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C73" s="23"/>
+      <c r="D73" s="24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B74" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="30" t="s">
+      <c r="C74" s="19"/>
+      <c r="D74" s="21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B75" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="C73" s="28"/>
-      <c r="D73" s="30" t="s">
+      <c r="C75" s="19"/>
+      <c r="D75" s="21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B74" s="12" t="s">
+      <c r="B76" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C74" s="28"/>
-      <c r="D74" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B75" s="12" t="s">
+      <c r="B77" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C75" s="28"/>
-      <c r="D75" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="C77" s="19"/>
+      <c r="D77" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="31"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
+      <c r="B79" s="27"/>
+      <c r="C79" s="27"/>
+      <c r="D79" s="28"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B80" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="26" t="s">
+      <c r="C80" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D78" s="26" t="s">
+      <c r="D80" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B79" s="12" t="s">
+      <c r="B81" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C79" s="28"/>
-      <c r="D79" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+      <c r="C81" s="19"/>
+      <c r="D81" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B82" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C80" s="28"/>
-      <c r="D80" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+      <c r="C82" s="19"/>
+      <c r="D82" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B83" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C81" s="28"/>
-      <c r="D81" s="30" t="s">
+      <c r="C83" s="19"/>
+      <c r="D83" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
+    <row r="85" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B83" s="17"/>
-      <c r="C83" s="17"/>
-      <c r="D83" s="17"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="9" t="s">
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B86" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C84" s="26" t="s">
+      <c r="C86" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D84" s="26" t="s">
+      <c r="D86" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B87" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C85" s="28"/>
-      <c r="D85" s="30" t="s">
+      <c r="C87" s="19"/>
+      <c r="D87" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="B91" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="C91" s="23"/>
+      <c r="D91" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B92" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" s="23"/>
+      <c r="D92" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="B93" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="C93" s="23"/>
+      <c r="D93" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="B94" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C94" s="23"/>
+      <c r="D94" s="24" t="s">
         <v>208</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A60:D60"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A77:D77"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A59:D59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2153,10 +2338,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="30"/>
       <c r="D1" s="1" t="s">
         <v>157</v>
       </c>
@@ -2229,10 +2414,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="20"/>
+      <c r="B11" s="30"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2294,10 +2479,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="20"/>
+      <c r="B20" s="30"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2343,10 +2528,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="32"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2416,10 +2601,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B37" s="23"/>
+      <c r="B37" s="34"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2468,10 +2653,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="25"/>
+      <c r="B44" s="32"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -2517,10 +2702,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
+      <c r="A51" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="20"/>
+      <c r="B51" s="30"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -2566,10 +2751,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="20"/>
+      <c r="B58" s="30"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -2607,10 +2792,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="B64" s="20"/>
+      <c r="B64" s="30"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -2656,10 +2841,10 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B71" s="20"/>
+      <c r="B71" s="30"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -2713,10 +2898,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="20"/>
+      <c r="B79" s="30"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -2754,10 +2939,10 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B85" s="20"/>
+      <c r="B85" s="30"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -2795,10 +2980,10 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="B91" s="20"/>
+      <c r="B91" s="30"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
@@ -2844,10 +3029,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="20" t="s">
+      <c r="A98" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="20"/>
+      <c r="B98" s="30"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
@@ -2893,10 +3078,10 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="20" t="s">
+      <c r="A105" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="B105" s="20"/>
+      <c r="B105" s="30"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
@@ -2926,10 +3111,10 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="22" t="s">
+      <c r="A110" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B110" s="23"/>
+      <c r="B110" s="34"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
@@ -2994,10 +3179,10 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="20" t="s">
+      <c r="A119" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B119" s="20"/>
+      <c r="B119" s="30"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
@@ -3051,10 +3236,10 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="21" t="s">
+      <c r="A127" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B127" s="21"/>
+      <c r="B127" s="35"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
@@ -3093,6 +3278,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A110:B110"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
@@ -3106,11 +3296,6 @@
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A110:B110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Split _14psticide_type. Updated data dictionary.
</commit_message>
<xml_diff>
--- a/docs/app_data_dictionary_20180713.xlsx
+++ b/docs/app_data_dictionary_20180713.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="233">
   <si>
     <t>_plotno</t>
   </si>
@@ -718,6 +718,12 @@
   </si>
   <si>
     <t>Date (yyyy-mm-dd), but defaults to (mm/dd/yyyy) when opened in Excel</t>
+  </si>
+  <si>
+    <t>_14pstcide_type_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of pesticide (splitted from _14psticide_type) </t>
   </si>
 </sst>
 </file>
@@ -924,6 +930,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -933,47 +963,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1255,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43:C44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,10 +1276,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1342,10 +1348,10 @@
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="35"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -1487,16 +1493,16 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="B20" s="39" t="s">
+      <c r="B20" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="40" t="s">
+      <c r="C20" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="31" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1506,10 +1512,10 @@
       <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="35"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -1673,24 +1679,24 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19" t="s">
+    <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19" t="s">
@@ -1698,99 +1704,99 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="C38" s="19"/>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+      <c r="D38" s="19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="19"/>
+      <c r="D39" s="21"/>
+    </row>
+    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="27"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="B40" s="35"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C41" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D41" s="17" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>67</v>
+        <v>211</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="42" t="s">
-        <v>230</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C43" s="19"/>
       <c r="D43" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B45" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C45" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="D44" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="19"/>
       <c r="D45" s="21" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="21" t="s">
@@ -1798,47 +1804,47 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>74</v>
+      </c>
       <c r="C47" s="19"/>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
+      <c r="D47" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="19"/>
+      <c r="D48" s="21"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="27"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="B49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C50" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D50" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B51" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="C51" s="19"/>
       <c r="D51" s="21" t="s">
@@ -1847,34 +1853,34 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C52" s="19"/>
       <c r="D52" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C53" s="19"/>
       <c r="D53" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C54" s="19"/>
       <c r="D54" s="21" t="s">
@@ -1883,34 +1889,34 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C55" s="19"/>
       <c r="D55" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="C56" s="19"/>
       <c r="D56" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C57" s="19"/>
       <c r="D57" s="21" t="s">
@@ -1919,80 +1925,80 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C58" s="19"/>
       <c r="D58" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B62" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C62" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D62" s="17" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="C63" s="19"/>
       <c r="D63" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C65" s="19"/>
       <c r="D65" s="21" t="s">
@@ -2001,10 +2007,10 @@
     </row>
     <row r="66" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" s="19"/>
       <c r="D66" s="21" t="s">
@@ -2013,22 +2019,22 @@
     </row>
     <row r="67" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" s="19"/>
       <c r="D67" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C68" s="19"/>
       <c r="D68" s="21" t="s">
@@ -2037,10 +2043,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C69" s="19"/>
       <c r="D69" s="21" t="s">
@@ -2049,10 +2055,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C70" s="19"/>
       <c r="D70" s="21" t="s">
@@ -2061,128 +2067,128 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C71" s="19"/>
       <c r="D71" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C72" s="19"/>
       <c r="D72" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
+    <row r="74" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="B74" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="C73" s="23"/>
-      <c r="D73" s="24" t="s">
+      <c r="C74" s="23"/>
+      <c r="D74" s="24" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="B74" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="21" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
-        <v>131</v>
+        <v>214</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>132</v>
+        <v>215</v>
       </c>
       <c r="C75" s="19"/>
       <c r="D75" s="21" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C76" s="19"/>
       <c r="D76" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C77" s="19"/>
       <c r="D77" s="21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="26" t="s">
+    <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="28"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="9" t="s">
+      <c r="B80" s="35"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="36"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B81" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="C81" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D80" s="17" t="s">
+      <c r="D81" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+    <row r="82" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B82" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="C81" s="19"/>
-      <c r="D81" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>148</v>
       </c>
       <c r="C82" s="19"/>
       <c r="D82" s="21" t="s">
@@ -2191,90 +2197,90 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C83" s="19"/>
       <c r="D83" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" s="19"/>
+      <c r="D84" s="21" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="29" t="s">
+    <row r="86" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A86" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="9" t="s">
+      <c r="B86" s="33"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="33"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B87" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="C87" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D86" s="17" t="s">
+      <c r="D87" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="10" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B87" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C87" s="19"/>
-      <c r="D87" s="21" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="29" t="s">
+      <c r="C88" s="19"/>
+      <c r="D88" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="B89" s="29"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="29"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="9" t="s">
+      <c r="B90" s="33"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B90" s="11" t="s">
+      <c r="B91" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C91" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="D90" s="17" t="s">
+      <c r="D91" s="17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="36" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B91" s="37" t="s">
+      <c r="B92" s="27" t="s">
         <v>224</v>
-      </c>
-      <c r="C91" s="23"/>
-      <c r="D91" s="24" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="B92" s="37" t="s">
-        <v>225</v>
       </c>
       <c r="C92" s="23"/>
       <c r="D92" s="24" t="s">
@@ -2282,11 +2288,11 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="36" t="s">
-        <v>226</v>
-      </c>
-      <c r="B93" s="37" t="s">
-        <v>228</v>
+      <c r="A93" s="26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>225</v>
       </c>
       <c r="C93" s="23"/>
       <c r="D93" s="24" t="s">
@@ -2294,27 +2300,39 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="B94" s="37" t="s">
-        <v>229</v>
+      <c r="A94" s="26" t="s">
+        <v>226</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="C94" s="23"/>
       <c r="D94" s="24" t="s">
         <v>208</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C95" s="23"/>
+      <c r="D95" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A61:D61"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2338,10 +2356,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="37"/>
       <c r="D1" s="1" t="s">
         <v>157</v>
       </c>
@@ -2414,10 +2432,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="37"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2479,10 +2497,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B20" s="30"/>
+      <c r="B20" s="37"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2528,10 +2546,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="B27" s="32"/>
+      <c r="B27" s="42"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -2601,10 +2619,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="B37" s="34"/>
+      <c r="B37" s="40"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -2653,10 +2671,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="32"/>
+      <c r="B44" s="42"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -2702,10 +2720,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="30" t="s">
+      <c r="A51" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="30"/>
+      <c r="B51" s="37"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -2751,10 +2769,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="30" t="s">
+      <c r="A58" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="30"/>
+      <c r="B58" s="37"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -2792,10 +2810,10 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="30" t="s">
+      <c r="A64" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="B64" s="30"/>
+      <c r="B64" s="37"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -2841,10 +2859,10 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="30" t="s">
+      <c r="A71" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B71" s="30"/>
+      <c r="B71" s="37"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -2898,10 +2916,10 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="30" t="s">
+      <c r="A79" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="B79" s="30"/>
+      <c r="B79" s="37"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -2939,10 +2957,10 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B85" s="30"/>
+      <c r="B85" s="37"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -2980,10 +2998,10 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="B91" s="30"/>
+      <c r="B91" s="37"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
@@ -3029,10 +3047,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="30" t="s">
+      <c r="A98" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="B98" s="30"/>
+      <c r="B98" s="37"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
@@ -3078,10 +3096,10 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="30" t="s">
+      <c r="A105" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B105" s="30"/>
+      <c r="B105" s="37"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
@@ -3111,10 +3129,10 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B110" s="34"/>
+      <c r="B110" s="40"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
@@ -3179,10 +3197,10 @@
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="30" t="s">
+      <c r="A119" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="B119" s="30"/>
+      <c r="B119" s="37"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
@@ -3236,10 +3254,10 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="35" t="s">
+      <c r="A127" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="B127" s="35"/>
+      <c r="B127" s="38"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
@@ -3278,11 +3296,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A110:B110"/>
     <mergeCell ref="A91:B91"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A11:B11"/>
@@ -3296,6 +3309,11 @@
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A110:B110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>